<commit_message>
3 week of August
</commit_message>
<xml_diff>
--- a/Stocktracking.xlsx
+++ b/Stocktracking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amitr\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63F10CE7-D2DF-4A35-BE8A-DD2EFC7D29BB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4E8E8A8-2DAA-4E9C-99FF-615A9DF072A9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DDC7E09A-D33A-4AF5-ADFB-31C781797254}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{DDC7E09A-D33A-4AF5-ADFB-31C781797254}"/>
   </bookViews>
   <sheets>
     <sheet name="Year" sheetId="1" r:id="rId1"/>
@@ -162,7 +162,29 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="31">
+  <dxfs count="20">
+    <dxf>
+      <numFmt numFmtId="21" formatCode="d\-mmm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="21" formatCode="d\-mmm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="21" formatCode="d\-mmm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="21" formatCode="d\-mmm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="21" formatCode="d\-mmm"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -171,6 +193,24 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
@@ -180,7 +220,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -194,7 +234,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -208,28 +248,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -239,102 +258,6 @@
           <bgColor theme="9" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="21" formatCode="d\-mmm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="21" formatCode="d\-mmm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="21" formatCode="d\-mmm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="21" formatCode="d\-mmm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="21" formatCode="d\-mmm"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -361,22 +284,22 @@
     <tableColumn id="6" xr3:uid="{A1A4CAAD-DDDC-4126-A0C5-62FC3151DD44}" name="May"/>
     <tableColumn id="7" xr3:uid="{859DF0FA-7EF6-41A8-A95E-EE1F55F08F31}" name="June"/>
     <tableColumn id="8" xr3:uid="{DE8AF5A6-040E-4B8A-88F5-7AFE67D5DD20}" name="July"/>
-    <tableColumn id="9" xr3:uid="{EBD36669-F84C-4143-BEB1-3A84924332EE}" name="August" dataDxfId="29">
+    <tableColumn id="9" xr3:uid="{EBD36669-F84C-4143-BEB1-3A84924332EE}" name="August" dataDxfId="12">
       <calculatedColumnFormula>'Months 2019'!C33</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{E302FDA9-1383-4996-9FED-4FD410E6AFDC}" name="September" dataDxfId="28">
+    <tableColumn id="10" xr3:uid="{E302FDA9-1383-4996-9FED-4FD410E6AFDC}" name="September" dataDxfId="11">
       <calculatedColumnFormula>'Months 2019'!F32</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{2F47FD48-9CE5-49F6-ACE7-4A7F09465C39}" name="October" dataDxfId="27">
+    <tableColumn id="11" xr3:uid="{2F47FD48-9CE5-49F6-ACE7-4A7F09465C39}" name="October" dataDxfId="10">
       <calculatedColumnFormula>'Months 2019'!I33</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{41A2CBF5-A427-46F0-85B4-9E1580702D7C}" name="November" dataDxfId="26">
+    <tableColumn id="12" xr3:uid="{41A2CBF5-A427-46F0-85B4-9E1580702D7C}" name="November" dataDxfId="9">
       <calculatedColumnFormula>'Months 2019'!L32</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{F1E8C364-A13E-4AF5-B5CB-904C0DA288F2}" name="December" dataDxfId="25">
+    <tableColumn id="13" xr3:uid="{F1E8C364-A13E-4AF5-B5CB-904C0DA288F2}" name="December" dataDxfId="8">
       <calculatedColumnFormula>'Months 2019'!O33</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{E79E9F41-0FAF-442A-A757-F5FC42B7A567}" name="Total " dataDxfId="20">
+    <tableColumn id="14" xr3:uid="{E79E9F41-0FAF-442A-A757-F5FC42B7A567}" name="Total " dataDxfId="7">
       <calculatedColumnFormula>SUM(C3:N3)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -388,7 +311,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{65B3CF1F-7532-4511-A243-BE899153EA71}" name="Table2" displayName="Table2" ref="B1:C33" totalsRowShown="0">
   <autoFilter ref="B1:C33" xr:uid="{91FCBC72-ABD2-4AA8-90B6-740F2D1CFE70}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{8421CE93-93FF-4F10-8CA3-6942058EC290}" name="Date " dataDxfId="24"/>
+    <tableColumn id="1" xr3:uid="{8421CE93-93FF-4F10-8CA3-6942058EC290}" name="Date " dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{E66A8DEC-6C9B-4B80-A436-2D6EC00C0ADA}" name="Amount"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -399,7 +322,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6DC94A07-EB3C-4351-8422-AD7834F4A89C}" name="Table3" displayName="Table3" ref="E1:F32" totalsRowShown="0">
   <autoFilter ref="E1:F32" xr:uid="{3A4DE990-0A76-4C15-B80A-7D027D23E0A4}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{5DEBFB13-0481-4E26-B508-31F0981BD28F}" name="Date" dataDxfId="23"/>
+    <tableColumn id="1" xr3:uid="{5DEBFB13-0481-4E26-B508-31F0981BD28F}" name="Date" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{AC439E4B-DD2A-47AC-9733-27368679FF5A}" name="Amount"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -410,7 +333,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{2BEAD29E-EBE2-4C32-AF36-6621ADED769B}" name="Table4" displayName="Table4" ref="H1:I33" totalsRowShown="0">
   <autoFilter ref="H1:I33" xr:uid="{B626C09E-46B3-4589-87F6-782ADF9EF19B}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{F2D6F05F-DFB9-4EE4-9E07-37C78F4E354C}" name="Date " dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{F2D6F05F-DFB9-4EE4-9E07-37C78F4E354C}" name="Date " dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{062927D3-BAC5-4A97-BB11-C91FB3285660}" name="Amount"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -421,7 +344,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{754959F5-A504-4AA5-8791-A8F62D6FECA5}" name="Table5" displayName="Table5" ref="K1:L32" totalsRowShown="0">
   <autoFilter ref="K1:L32" xr:uid="{9653BE01-BD89-4850-B7CC-18E45CD7BE00}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{A3C13AD5-096D-4B65-8581-19528EF0021F}" name="Date" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{A3C13AD5-096D-4B65-8581-19528EF0021F}" name="Date" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{A4334E7F-A3DB-4A0B-A68D-0B9F37291CDE}" name="Amount"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -432,7 +355,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{8CBABE50-78BA-4413-ABF6-6F38B4212567}" name="Table6" displayName="Table6" ref="N1:O33" totalsRowShown="0">
   <autoFilter ref="N1:O33" xr:uid="{C0D5ABBB-14A0-4408-A9BF-D169160DFE03}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{FDED5317-1876-470B-AB34-E02B07E9B7F4}" name="Date" dataDxfId="30"/>
+    <tableColumn id="1" xr3:uid="{FDED5317-1876-470B-AB34-E02B07E9B7F4}" name="Date" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{36C8DF08-7CEB-4D52-9CE6-9455DF253EA2}" name="Amount"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -749,7 +672,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC51C81E-1236-4588-85C9-5552041ECFF9}">
   <dimension ref="B2:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
@@ -835,7 +758,7 @@
       </c>
       <c r="J3">
         <f>'Months 2019'!C33</f>
-        <v>-11881</v>
+        <v>-3614</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -854,7 +777,7 @@
       </c>
       <c r="O3" s="5">
         <f t="shared" ref="O3:O7" si="0">SUM(C3:N3)</f>
-        <v>-11881</v>
+        <v>-3614</v>
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
@@ -907,19 +830,19 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:O3">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="17" priority="5" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="16" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="15" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -935,8 +858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39A702FE-6BE9-4C1E-946B-561928870A3A}">
   <dimension ref="B1:T33"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O26" sqref="O26"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1243,6 +1166,9 @@
       <c r="S10">
         <v>86</v>
       </c>
+      <c r="T10">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
@@ -1580,7 +1506,7 @@
         <v>43699</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>4979</v>
       </c>
       <c r="E23" s="2">
         <v>43730</v>
@@ -1608,6 +1534,9 @@
       <c r="B24" s="2">
         <v>43700</v>
       </c>
+      <c r="C24">
+        <v>3288</v>
+      </c>
       <c r="E24" s="2">
         <v>43731</v>
       </c>
@@ -1841,7 +1770,7 @@
       </c>
       <c r="C33">
         <f>SUM(C2:C31)</f>
-        <v>-11881</v>
+        <v>-3614</v>
       </c>
       <c r="H33" t="s">
         <v>17</v>
@@ -1861,12 +1790,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:P33">
-    <cfRule type="cellIs" dxfId="17" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C33">
-    <cfRule type="cellIs" dxfId="15" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>